<commit_message>
mobile ready draft 1
</commit_message>
<xml_diff>
--- a/gt_mit_buttons/data.xlsx
+++ b/gt_mit_buttons/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelmerk/Meine Ablage/Uni_gdrive/Sandbox/HeatmapStudy/gt_mit_buttons/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sarah/Documents/Projekte/06_Heatmap-Studien/Studie 2/shiny approach/HeatmapStudy/gt_mit_buttons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15973414-B230-DF42-BFDB-55BF8AE4DDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D1CD2E-61DE-644D-8ACB-52F5D586DC28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="28640" windowHeight="21440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19940" yWindow="500" windowWidth="14980" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>Imperativ erkennen e)</t>
   </si>
   <si>
-    <t>Indikativ erkennen f)</t>
-  </si>
-  <si>
     <t>Indikativ erkennen a)</t>
   </si>
   <si>
@@ -146,10 +143,13 @@
     <t>Konjunktiv erkennen e)</t>
   </si>
   <si>
-    <t>Konjunktiv 2 bilden II c)</t>
-  </si>
-  <si>
     <t>Schüler:in</t>
+  </si>
+  <si>
+    <t>Indikativ erkennen e)</t>
+  </si>
+  <si>
+    <t>Konjunktiv II bilden c)</t>
   </si>
 </sst>
 </file>
@@ -510,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="172" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -551,37 +551,37 @@
         <v>27</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="M1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">

</xml_diff>